<commit_message>
add print qr code, generate code instantly, adjust barcode location to db location
</commit_message>
<xml_diff>
--- a/database/data.xlsx
+++ b/database/data.xlsx
@@ -517,7 +517,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -545,24 +545,24 @@
         <v>qrCodePath</v>
       </c>
       <c r="H1" t="str">
+        <v>barcodePath</v>
+      </c>
+      <c r="I1" t="str">
+        <v>barcodeType</v>
+      </c>
+      <c r="J1" t="str">
         <v>createdAt</v>
       </c>
-      <c r="I1" t="str">
+      <c r="K1" t="str">
         <v>updatedAt</v>
-      </c>
-      <c r="J1" t="str">
-        <v>barcodePath</v>
-      </c>
-      <c r="K1" t="str">
-        <v>barcodeType</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>50de4f4f-b9a6-43d8-a74e-3996ca98b4ab</v>
+        <v>dba28441-3044-46f2-a914-204bf9fd0954</v>
       </c>
       <c r="B2" t="str">
-        <v>Gear Motor 123</v>
+        <v>Test</v>
       </c>
       <c r="C2" t="str">
         <v>Buah</v>
@@ -571,170 +571,30 @@
         <v>123</v>
       </c>
       <c r="E2">
-        <v>5123</v>
+        <v>123</v>
       </c>
       <c r="F2" t="str">
-        <v>GM1</v>
+        <v>T</v>
       </c>
       <c r="G2" t="str">
-        <v>D:\Project\Developments\inventory\qr-codes\product_50de4f4f-b9a6-43d8-a74e-3996ca98b4ab.png</v>
+        <v>D:\Project\Developments\inventory\database\images\qr_T.png</v>
       </c>
       <c r="H2" t="str">
-        <v>2025-07-01T15:54:12.837Z</v>
+        <v>D:\Project\Developments\inventory\database\images\barcode_T.png</v>
       </c>
       <c r="I2" t="str">
-        <v>2025-07-01T17:44:44.600Z</v>
+        <v>code128</v>
       </c>
       <c r="J2" t="str">
-        <v>D:\Project\Developments\inventory\qr-codes\barcode_50de4f4f-b9a6-43d8-a74e-3996ca98b4ab.png</v>
+        <v>2025-07-01T18:13:10.810Z</v>
       </c>
       <c r="K2" t="str">
-        <v>code128</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>11d3be62-d066-4854-913d-f446852117e1</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Gear Motor 123</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Buah</v>
-      </c>
-      <c r="D3">
-        <v>123</v>
-      </c>
-      <c r="E3">
-        <v>122</v>
-      </c>
-      <c r="F3" t="str">
-        <v>GM1-2</v>
-      </c>
-      <c r="G3" t="str">
-        <v>D:\Project\Developments\inventory\qr-codes\product_11d3be62-d066-4854-913d-f446852117e1.png</v>
-      </c>
-      <c r="H3" t="str">
-        <v>2025-07-01T15:54:30.021Z</v>
-      </c>
-      <c r="I3" t="str">
-        <v>2025-07-01T17:44:54.577Z</v>
-      </c>
-      <c r="J3" t="str">
-        <v>D:\Project\Developments\inventory\qr-codes\barcode_11d3be62-d066-4854-913d-f446852117e1.png</v>
-      </c>
-      <c r="K3" t="str">
-        <v>code128</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>2eb9ed12-9886-4a60-b530-30210d44385e</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Gear</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Buah</v>
-      </c>
-      <c r="D4">
-        <v>12312</v>
-      </c>
-      <c r="E4">
-        <v>123</v>
-      </c>
-      <c r="F4" t="str">
-        <v>G</v>
-      </c>
-      <c r="G4" t="str">
-        <v>D:\Project\Developments\inventory\qr-codes\product_2eb9ed12-9886-4a60-b530-30210d44385e.png</v>
-      </c>
-      <c r="H4" t="str">
-        <v>2025-07-01T16:03:52.149Z</v>
-      </c>
-      <c r="I4" t="str">
-        <v>2025-07-01T17:44:51.192Z</v>
-      </c>
-      <c r="J4" t="str">
-        <v>D:\Project\Developments\inventory\qr-codes\barcode_2eb9ed12-9886-4a60-b530-30210d44385e.png</v>
-      </c>
-      <c r="K4" t="str">
-        <v>code128</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>c49bddeb-49c7-425d-9da8-27d282e1bfad</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Produk Baru</v>
-      </c>
-      <c r="C5" t="str">
-        <v>test</v>
-      </c>
-      <c r="D5">
-        <v>123</v>
-      </c>
-      <c r="E5">
-        <v>123</v>
-      </c>
-      <c r="F5" t="str">
-        <v>PB</v>
-      </c>
-      <c r="G5" t="str">
-        <v>D:\Project\Developments\inventory\qr-codes\product_c49bddeb-49c7-425d-9da8-27d282e1bfad.png</v>
-      </c>
-      <c r="H5" t="str">
-        <v>2025-07-01T17:35:26.909Z</v>
-      </c>
-      <c r="I5" t="str">
-        <v>2025-07-01T17:44:27.080Z</v>
-      </c>
-      <c r="J5" t="str">
-        <v>D:\Project\Developments\inventory\qr-codes\barcode_c49bddeb-49c7-425d-9da8-27d282e1bfad.png</v>
-      </c>
-      <c r="K5" t="str">
-        <v>code128</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>e42f8c2d-4e4b-4dce-9d23-511ffbe60e90</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Product 2</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Buah</v>
-      </c>
-      <c r="D6">
-        <v>123</v>
-      </c>
-      <c r="E6">
-        <v>123</v>
-      </c>
-      <c r="F6" t="str">
-        <v>P2</v>
-      </c>
-      <c r="G6" t="str">
-        <v>D:\Project\Developments\inventory\qr-codes\product_e42f8c2d-4e4b-4dce-9d23-511ffbe60e90.png</v>
-      </c>
-      <c r="H6" t="str">
-        <v>2025-07-01T17:43:40.938Z</v>
-      </c>
-      <c r="I6" t="str">
-        <v>2025-07-01T17:44:15.672Z</v>
-      </c>
-      <c r="J6" t="str">
-        <v>D:\Project\Developments\inventory\qr-codes\barcode_e42f8c2d-4e4b-4dce-9d23-511ffbe60e90.png</v>
-      </c>
-      <c r="K6" t="str">
-        <v>code128</v>
+        <v>2025-07-01T18:22:09.531Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>